<commit_message>
remove calibration and add partial vesting
</commit_message>
<xml_diff>
--- a/Inputs_riskSharing/RunControl_riskSharing.xlsx
+++ b/Inputs_riskSharing/RunControl_riskSharing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\PenSim-Projects\Model_Main\Inputs_riskSharing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4807B6-A2A1-4063-BE8A-2D766E22F2D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2383E240-584B-4822-98C3-B8F6671F6DC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="362">
   <si>
     <t>Sheet #</t>
   </si>
@@ -1159,6 +1159,12 @@
   </si>
   <si>
     <t>riskShaing_demographics_bf.5_100y</t>
+  </si>
+  <si>
+    <t>term.average2</t>
+  </si>
+  <si>
+    <t>average of 4 plans</t>
   </si>
 </sst>
 </file>
@@ -2135,7 +2141,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2620,7 +2626,7 @@
         <v>167</v>
       </c>
       <c r="O6" s="31" t="s">
-        <v>211</v>
+        <v>360</v>
       </c>
       <c r="P6" s="31" t="s">
         <v>198</v>
@@ -2632,8 +2638,7 @@
         <v>0</v>
       </c>
       <c r="S6" s="46">
-        <f>2.2%*1.461</f>
-        <v>3.2142000000000004E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="T6" s="31">
         <v>3</v>
@@ -2780,7 +2785,7 @@
         <v>167</v>
       </c>
       <c r="O7" s="31" t="s">
-        <v>211</v>
+        <v>360</v>
       </c>
       <c r="P7" s="31" t="s">
         <v>198</v>
@@ -2792,8 +2797,7 @@
         <v>0</v>
       </c>
       <c r="S7" s="46">
-        <f>2.2%*1.461</f>
-        <v>3.2142000000000004E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="T7" s="31">
         <v>3</v>
@@ -2942,7 +2946,7 @@
         <v>167</v>
       </c>
       <c r="O8" s="31" t="s">
-        <v>211</v>
+        <v>360</v>
       </c>
       <c r="P8" s="31" t="s">
         <v>198</v>
@@ -2954,8 +2958,7 @@
         <v>0</v>
       </c>
       <c r="S8" s="46">
-        <f>2.2%*1.461*0.5</f>
-        <v>1.6071000000000002E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="T8" s="31">
         <v>3</v>
@@ -8831,7 +8834,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000016000000}">
           <x14:formula1>
-            <xm:f>DropDowns!$A$64:$A$71</xm:f>
+            <xm:f>DropDowns!$A$64:$A$72</xm:f>
           </x14:formula1>
           <xm:sqref>O13:O54 O6:O8</xm:sqref>
         </x14:dataValidation>
@@ -8855,7 +8858,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-00001A000000}">
           <x14:formula1>
-            <xm:f>DropDowns!$A$74:$A$77</xm:f>
+            <xm:f>DropDowns!$A$75:$A$78</xm:f>
           </x14:formula1>
           <xm:sqref>P13:P54 P6:P8</xm:sqref>
         </x14:dataValidation>
@@ -9163,10 +9166,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9491,76 +9494,84 @@
       <c r="A64" s="23" t="s">
         <v>211</v>
       </c>
+      <c r="C64" t="s">
+        <v>151</v>
+      </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>180</v>
-      </c>
-      <c r="C65" t="s">
-        <v>151</v>
+    <row r="65" spans="1:3" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="23" t="s">
+        <v>360</v>
+      </c>
+      <c r="C65" s="23" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>111</v>
+        <v>194</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>168</v>
+        <v>111</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="73" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="14" t="s">
+    <row r="74" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="14" t="s">
         <v>181</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>198</v>
-      </c>
-      <c r="C74" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="C75" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C76" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>182</v>
+      </c>
+      <c r="C77" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>180</v>
       </c>
     </row>
@@ -9577,7 +9588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AR40"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>

</xml_diff>